<commit_message>
add performance summary with hartford
</commit_message>
<xml_diff>
--- a/results/summary_tables/Descriptive Comparison - Hartford.xlsx
+++ b/results/summary_tables/Descriptive Comparison - Hartford.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollywiberg/Dropbox (MIT)/COVID_risk/covid19_calculator/results/summary_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{85847719-78F7-4F45-9BE0-95A4A71BD91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1288F7-69F3-C745-9358-C376819A3869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16580"/>
+    <workbookView xWindow="1260" yWindow="460" windowWidth="21140" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="descriptive_derivation_hartford" sheetId="1" r:id="rId1"/>
@@ -20,29 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
   <si>
     <t>index</t>
   </si>
   <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>Percent Missing</t>
   </si>
   <si>
-    <t>Output_A</t>
-  </si>
-  <si>
-    <t>Percent Missing_A</t>
-  </si>
-  <si>
-    <t>Output_B</t>
-  </si>
-  <si>
-    <t>Percent Missing_B</t>
-  </si>
-  <si>
     <t>p-Value</t>
   </si>
   <si>
@@ -262,33 +247,6 @@
     <t>288.0 (52.17%)</t>
   </si>
   <si>
-    <t>Cardiac dysrhythmias</t>
-  </si>
-  <si>
-    <t>200.0 (7.06%)</t>
-  </si>
-  <si>
-    <t>nan (nan%)</t>
-  </si>
-  <si>
-    <t>Chronic kidney disease</t>
-  </si>
-  <si>
-    <t>65.0 (2.3%)</t>
-  </si>
-  <si>
-    <t>Coronary atherosclerosis and other heart disease</t>
-  </si>
-  <si>
-    <t>125.0 (4.42%)</t>
-  </si>
-  <si>
-    <t>Diabetes</t>
-  </si>
-  <si>
-    <t>345.0 (12.19%)</t>
-  </si>
-  <si>
     <t>Patient Count</t>
   </si>
   <si>
@@ -302,12 +260,15 @@
   </si>
   <si>
     <t>Hartford</t>
+  </si>
+  <si>
+    <t>Median (IQR)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -625,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -745,25 +706,109 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -773,7 +818,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -781,12 +826,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -797,7 +853,18 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -847,29 +914,34 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1224,11 +1296,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1244,637 +1316,533 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="2"/>
+      <c r="A1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="12">
+      <c r="A2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="4">
         <v>3383</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="12">
+      <c r="C2" s="5"/>
+      <c r="D2" s="4">
         <v>2831</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="12">
+      <c r="E2" s="5"/>
+      <c r="F2" s="4">
         <v>552</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="7"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0.200616900874068</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C5" s="3">
+        <v>0.1502</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10">
+      <c r="E5" s="3">
+        <v>0.17910000000000001</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.8E-3</v>
+      </c>
+      <c r="H5" s="13">
+        <v>5.3798605220621003E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>7.0599999999999996E-2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3">
+        <v>8.3699999999999997E-2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="H6" s="14">
+        <v>4.1878750175201698E-24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.1091</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.10630000000000001</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.1232</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0.83852269776797494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4.1399999999999999E-2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="H8" s="14">
+        <v>5.8297331664264503E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4.1700000000000001E-2</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0.29736171906332998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.3599999999999999E-2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="3">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="H10" s="13">
+        <v>2.4048400397206899E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="3">
+        <v>6.1800000000000001E-2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1.8E-3</v>
+      </c>
+      <c r="H11" s="14">
+        <v>1.2156880759487099E-49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.10050000000000001</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.40039999999999998</v>
+      </c>
+      <c r="H12" s="13">
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="10">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.113</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="H13" s="14">
+        <v>1.8970298600384201E-44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.1026</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.1169</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0.36430922053762799</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="3">
+        <v>9.9299999999999999E-2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.113</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H15" s="14">
+        <v>1.08865383950573E-10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.12770000000000001</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.12820000000000001</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="H16" s="13">
+        <v>0.14691506502264501</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="3">
+        <v>9.9900000000000003E-2</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.113</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3.2599999999999997E-2</v>
+      </c>
+      <c r="H17" s="13">
+        <v>1.7986211590975101E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="3">
+        <v>6.1499999999999999E-2</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="3">
+        <v>6.7100000000000007E-2</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3.2599999999999997E-2</v>
+      </c>
+      <c r="H18" s="14">
+        <v>1.31903363460327E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="3">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="3">
+        <v>7.7399999999999997E-2</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="3">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="H19" s="13">
+        <v>0.92384792406916205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.30769999999999997</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.25219999999999998</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.59240000000000004</v>
+      </c>
+      <c r="H20" s="13">
+        <v>0.421648680372264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="17">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="10">
+      <c r="D21" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="17">
         <v>0</v>
       </c>
-      <c r="H4" s="4">
-        <v>0.200616900874068</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="10">
-        <v>0.1502</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0.17910000000000001</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="10">
-        <v>1.8E-3</v>
-      </c>
-      <c r="H5" s="4">
-        <v>5.3798605220621003E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="10">
-        <v>7.0599999999999996E-2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="10">
-        <v>8.3699999999999997E-2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="10">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="H6" s="5">
-        <v>4.1878750175201698E-24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="10">
-        <v>0.1091</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="10">
-        <v>0.10630000000000001</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="10">
-        <v>0.1232</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0.83852269776797494</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="10">
-        <v>4.1399999999999999E-2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="10">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="10">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="H8" s="5">
-        <v>5.8297331664264503E-6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="10">
-        <v>4.3200000000000002E-2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="10">
-        <v>4.3400000000000001E-2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="10">
-        <v>4.1700000000000001E-2</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0.29736171906332998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="10">
-        <v>7.3599999999999999E-2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="10">
-        <v>8.0199999999999994E-2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="10">
-        <v>3.9899999999999998E-2</v>
-      </c>
-      <c r="H10" s="4">
-        <v>2.4048400397206899E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="10">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="10">
-        <v>6.1800000000000001E-2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="10">
-        <v>1.8E-3</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1.2156880759487099E-49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="10">
-        <v>0.10050000000000001</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="10">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="10">
-        <v>0.40039999999999998</v>
-      </c>
-      <c r="H12" s="4">
+      <c r="F21" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="10">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="10">
-        <v>0.113</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="10">
-        <v>2.7199999999999998E-2</v>
-      </c>
-      <c r="H13" s="5">
-        <v>1.8970298600384201E-44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="10">
-        <v>0.1026</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="10">
-        <v>0.1169</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="10">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0.36430922053762799</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="10">
-        <v>9.9299999999999999E-2</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="10">
-        <v>0.113</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="10">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="H15" s="5">
-        <v>1.08865383950573E-10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="10">
-        <v>0.12770000000000001</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="10">
-        <v>0.12820000000000001</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="10">
-        <v>0.125</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0.14691506502264501</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="10">
-        <v>9.9900000000000003E-2</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="10">
-        <v>0.113</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="10">
-        <v>3.2599999999999997E-2</v>
-      </c>
-      <c r="H17" s="4">
-        <v>1.7986211590975101E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="10">
-        <v>6.1499999999999999E-2</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="10">
-        <v>6.7100000000000007E-2</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G18" s="10">
-        <v>3.2599999999999997E-2</v>
-      </c>
-      <c r="H18" s="5">
-        <v>1.31903363460327E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="10">
-        <v>7.3300000000000004E-2</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="10">
-        <v>7.7399999999999997E-2</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="10">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="H19" s="4">
-        <v>0.92384792406916205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="10">
-        <v>0.30769999999999997</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="10">
-        <v>0.25219999999999998</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="10">
-        <v>0.59240000000000004</v>
-      </c>
-      <c r="H20" s="4">
-        <v>0.421648680372264</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="10">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="10">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="10">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
+      <c r="H21" s="18">
         <v>8.3799601916066299E-9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="10">
-        <v>0.16320000000000001</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="10">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="10">
-        <v>1</v>
-      </c>
-      <c r="H22" s="4">
-        <v>0.99986014234545595</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="10">
-        <v>0.16320000000000001</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="10">
-        <v>0</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G23" s="10">
-        <v>1</v>
-      </c>
-      <c r="H23" s="4">
-        <v>0.99994795562749095</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="10">
-        <v>0.16320000000000001</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="10">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G24" s="10">
-        <v>1</v>
-      </c>
-      <c r="H24" s="4">
-        <v>0.99990680012907596</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="11">
-        <v>0.16320000000000001</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="11">
-        <v>0</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G25" s="11">
-        <v>1</v>
-      </c>
-      <c r="H25" s="7">
-        <v>0.99978128675480904</v>
       </c>
     </row>
   </sheetData>
@@ -1886,8 +1854,8 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="B2:C2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:H25">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="H4:H21">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>